<commit_message>
Adicionando link em cada artefato
</commit_message>
<xml_diff>
--- a/Gestão do Projeto/Indicadores/SumarioIndicadores.xlsx
+++ b/Gestão do Projeto/Indicadores/SumarioIndicadores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/Documents/GitHub/ips-brasil-documentos/Gestão do Projeto/Indicadores/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syola\Documents\ips-brasil-documentos\Gestão do Projeto\Indicadores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5716AE5A-9D1F-3445-AFB8-23029A1F094D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCB4585-3812-4603-9B9D-5CB3F98B2121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="2160" windowWidth="25320" windowHeight="11040" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sumario" sheetId="1" r:id="rId1"/>
@@ -28,28 +28,17 @@
     <sheet name="Composition" sheetId="11" r:id="rId13"/>
     <sheet name="Bundle" sheetId="12" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="164">
   <si>
     <t>Artefato</t>
   </si>
@@ -519,9 +508,6 @@
     <t>Mapa de Conceitos RNDS-&gt;</t>
   </si>
   <si>
-    <t>Nome (URL)</t>
-  </si>
-  <si>
     <t>SIM/Prórpio Value Set</t>
   </si>
   <si>
@@ -550,7 +536,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -659,7 +645,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -709,12 +695,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
-    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+    <cellStyle name="20% - Ênfase1" xfId="2" builtinId="30"/>
+    <cellStyle name="40% - Ênfase1" xfId="3" builtinId="31"/>
+    <cellStyle name="Ênfase1" xfId="1" builtinId="29"/>
+    <cellStyle name="Hiperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -25503,7 +25492,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -25805,16 +25794,16 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="47.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -25834,7 +25823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="2" customFormat="1">
       <c r="A2" s="5" t="s">
         <v>75</v>
       </c>
@@ -25858,7 +25847,7 @@
         <v>0.79365079365079361</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="3" customFormat="1">
       <c r="A3" s="4" t="s">
         <v>76</v>
       </c>
@@ -25882,7 +25871,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="2" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>77</v>
       </c>
@@ -25906,7 +25895,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="3" customFormat="1">
       <c r="A5" s="4" t="s">
         <v>78</v>
       </c>
@@ -25930,7 +25919,7 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="3" customFormat="1">
       <c r="A6" s="4" t="s">
         <v>153</v>
       </c>
@@ -25951,28 +25940,28 @@
         <v>0.93915343915343907</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" s="2" customFormat="1">
       <c r="A7" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B7" s="8">
         <v>1</v>
       </c>
-      <c r="C7" s="6" t="str">
+      <c r="C7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="D7" s="6" t="str">
+        <v>0.6</v>
+      </c>
+      <c r="D7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>0.42857142857142855</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.67619047619047612</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="3" customFormat="1">
       <c r="A8" s="4" t="s">
         <v>80</v>
       </c>
@@ -25981,11 +25970,11 @@
       </c>
       <c r="C8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>9.375E-2</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>9.375E-2</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="E8" s="6" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -25993,10 +25982,10 @@
       </c>
       <c r="F8" s="22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39583333333333331</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.35555555555555562</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="2" customFormat="1">
       <c r="A9" s="5" t="s">
         <v>150</v>
       </c>
@@ -26017,7 +26006,7 @@
         <v>0.4102564102564103</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="3" customFormat="1">
       <c r="A10" s="4" t="s">
         <v>81</v>
       </c>
@@ -26038,7 +26027,7 @@
         <v>0.39393939393939387</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" s="2" customFormat="1">
       <c r="A11" s="5" t="s">
         <v>151</v>
       </c>
@@ -26059,7 +26048,7 @@
         <v>0.55555555555555547</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" s="3" customFormat="1">
       <c r="A12" s="4" t="s">
         <v>82</v>
       </c>
@@ -26083,7 +26072,7 @@
         <v>1.9607843137254902E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" s="2" customFormat="1">
       <c r="A13" s="5" t="s">
         <v>152</v>
       </c>
@@ -26107,13 +26096,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" s="1" customFormat="1">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="21">
         <f ca="1">AVERAGE(F2:F13)</f>
-        <v>0.55622195297440391</v>
+        <v>0.52588134450879553</v>
       </c>
     </row>
   </sheetData>
@@ -26145,17 +26134,17 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="62.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="44.6640625" customWidth="1"/>
-    <col min="5" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="5" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -26181,7 +26170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="2" customFormat="1">
       <c r="A2" s="15" t="str">
         <f t="shared" ref="A2:A27" si="0">CONCATENATE(C2,"/",B2)</f>
         <v>CodeSystem/urn:ietf:bcp:47</v>
@@ -26204,7 +26193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" s="3" customFormat="1">
       <c r="A3" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/CommonLanguages</v>
@@ -26228,7 +26217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" s="2" customFormat="1">
       <c r="A4" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/Medication Status Codes</v>
@@ -26251,7 +26240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" s="3" customFormat="1">
       <c r="A5" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/Medication Status Codes</v>
@@ -26275,7 +26264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" s="2" customFormat="1">
       <c r="A6" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/SNOMEDCTDrugTherapyStatusCodes</v>
@@ -26297,7 +26286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" s="3" customFormat="1">
       <c r="A7" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/SNOMEDCTDrugTherapyStatusCodes</v>
@@ -26320,7 +26309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" s="2" customFormat="1">
       <c r="A8" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/Medication usage category codes</v>
@@ -26342,7 +26331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" s="3" customFormat="1">
       <c r="A9" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/Medication usage category codes</v>
@@ -26365,7 +26354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" s="2" customFormat="1">
       <c r="A10" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/MedicationSnomedCodesAbsentUnknown</v>
@@ -26387,7 +26376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" s="3" customFormat="1">
       <c r="A11" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/MedicationSnomedCodesAbsentUnknown</v>
@@ -26410,7 +26399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" s="2" customFormat="1">
       <c r="A12" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/ResourceType</v>
@@ -26432,7 +26421,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" s="3" customFormat="1">
       <c r="A13" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/ResourceType</v>
@@ -26455,7 +26444,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" s="2" customFormat="1">
       <c r="A14" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/Condition/Problem/DiagnosisCodes</v>
@@ -26477,7 +26466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" s="3" customFormat="1">
       <c r="A15" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/Condition/Problem/DiagnosisCodes</v>
@@ -26500,7 +26489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" s="2" customFormat="1">
       <c r="A16" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/SNOMEDCTAdditionalDosageInstructions</v>
@@ -26522,7 +26511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" s="3" customFormat="1">
       <c r="A17" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/SNOMEDCTAdditionalDosageInstructions</v>
@@ -26545,7 +26534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" s="2" customFormat="1">
       <c r="A18" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/SNOMEDCTMedicationAsNeededReasonCodes</v>
@@ -26567,7 +26556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" s="3" customFormat="1">
       <c r="A19" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/SNOMEDCTMedicationAsNeededReasonCodes</v>
@@ -26590,7 +26579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" s="2" customFormat="1">
       <c r="A20" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/SNOMEDCTAnatomicalStructureForAdministrationSiteCodes</v>
@@ -26612,7 +26601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" s="3" customFormat="1">
       <c r="A21" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/SNOMEDCTAnatomicalStructureForAdministrationSiteCodes</v>
@@ -26635,7 +26624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" s="2" customFormat="1">
       <c r="A22" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/MedicineRouteOfAdministrationUvIps</v>
@@ -26657,7 +26646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" s="3" customFormat="1">
       <c r="A23" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/MedicineRouteOfAdministrationUvIps</v>
@@ -26680,7 +26669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" s="2" customFormat="1">
       <c r="A24" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/SNOMEDCTAdministrationMethodCodes</v>
@@ -26702,7 +26691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" s="3" customFormat="1">
       <c r="A25" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/SNOMEDCTAdministrationMethodCodes</v>
@@ -26725,7 +26714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" s="2" customFormat="1">
       <c r="A26" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/DoseAndRateType</v>
@@ -26747,7 +26736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" s="3" customFormat="1">
       <c r="A27" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/DoseAndRateType</v>
@@ -26783,17 +26772,17 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="44.6640625" customWidth="1"/>
-    <col min="5" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="5" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -26819,7 +26808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="2" customFormat="1">
       <c r="A2" s="15" t="str">
         <f t="shared" ref="A2:A23" si="0">CONCATENATE(C2,"/",B2)</f>
         <v>CodeSystem/urn:ietf:bcp:47</v>
@@ -26842,7 +26831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" s="3" customFormat="1">
       <c r="A3" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/CommonLanguages</v>
@@ -26866,7 +26855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" s="2" customFormat="1">
       <c r="A4" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/MedicationSnomedCodesAbsentUnknown</v>
@@ -26889,7 +26878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" s="3" customFormat="1">
       <c r="A5" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/MedicationSnomedCodesAbsentUnknown</v>
@@ -26913,7 +26902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" s="2" customFormat="1">
       <c r="A6" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/Medications - SNOMED CT IPS Free Set</v>
@@ -26935,7 +26924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" s="3" customFormat="1">
       <c r="A7" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/Medications - SNOMED CT IPS Free Set</v>
@@ -26958,7 +26947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" s="2" customFormat="1">
       <c r="A8" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/WHO ATC - IPS</v>
@@ -26980,7 +26969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" s="3" customFormat="1">
       <c r="A9" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/WHO ATC - IPS</v>
@@ -27003,7 +26992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" s="2" customFormat="1">
       <c r="A10" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/Absent or Unknown Medication - IPS</v>
@@ -27025,7 +27014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" s="3" customFormat="1">
       <c r="A11" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/Absent or Unknown Medication - IPS</v>
@@ -27048,7 +27037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" s="2" customFormat="1">
       <c r="A12" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/Medication Status Codes</v>
@@ -27070,7 +27059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" s="3" customFormat="1">
       <c r="A13" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/Medication Status Codes</v>
@@ -27093,7 +27082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" s="2" customFormat="1">
       <c r="A14" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/MedicineDoseFormUvIps</v>
@@ -27115,7 +27104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" s="3" customFormat="1">
       <c r="A15" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/MedicineDoseFormUvIps</v>
@@ -27138,7 +27127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" s="2" customFormat="1">
       <c r="A16" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/MedicineActiveSubstancesUvIps</v>
@@ -27160,7 +27149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" s="3" customFormat="1">
       <c r="A17" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/MedicineActiveSubstancesUvIps</v>
@@ -27183,7 +27172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" s="2" customFormat="1">
       <c r="A18" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/</v>
@@ -27202,7 +27191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" s="3" customFormat="1">
       <c r="A19" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/</v>
@@ -27222,7 +27211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" s="2" customFormat="1">
       <c r="A20" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/</v>
@@ -27241,7 +27230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" s="3" customFormat="1">
       <c r="A21" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/</v>
@@ -27261,7 +27250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" s="2" customFormat="1">
       <c r="A22" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/</v>
@@ -27280,7 +27269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" s="3" customFormat="1">
       <c r="A23" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/</v>
@@ -27313,17 +27302,17 @@
       <selection activeCell="A14" sqref="A14:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="44.6640625" customWidth="1"/>
-    <col min="5" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="5" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -27349,7 +27338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="2" customFormat="1">
       <c r="A2" s="15" t="str">
         <f t="shared" ref="A2:A13" si="0">CONCATENATE(C2,"/",B2)</f>
         <v>CodeSystem/urn:ietf:bcp:47</v>
@@ -27372,7 +27361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" s="3" customFormat="1">
       <c r="A3" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/ CommonLanguages</v>
@@ -27396,7 +27385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" s="2" customFormat="1">
       <c r="A4" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/ObservationCategoryCodes</v>
@@ -27419,7 +27408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" s="3" customFormat="1">
       <c r="A5" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/ObservationCategoryCodes</v>
@@ -27443,7 +27432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" s="2" customFormat="1">
       <c r="A6" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/loinc.org</v>
@@ -27465,7 +27454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" s="3" customFormat="1">
       <c r="A7" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/observation-codes</v>
@@ -27488,7 +27477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" s="2" customFormat="1">
       <c r="A8" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/ DataAbsentReason</v>
@@ -27510,7 +27499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" s="3" customFormat="1">
       <c r="A9" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/ DataAbsentReason</v>
@@ -27533,7 +27522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" s="2" customFormat="1">
       <c r="A10" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/ ObservationInterpretationCodes</v>
@@ -27555,7 +27544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" s="3" customFormat="1">
       <c r="A11" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/ ObservationInterpretationCodes</v>
@@ -27578,7 +27567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" s="2" customFormat="1">
       <c r="A12" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/ ObservationReferenceRangeMeaningCodes</v>
@@ -27600,7 +27589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" s="3" customFormat="1">
       <c r="A13" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/ ObservationReferenceRangeMeaningCodes</v>
@@ -27636,17 +27625,17 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="44.6640625" customWidth="1"/>
-    <col min="5" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="5" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -27672,7 +27661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="2" customFormat="1">
       <c r="A2" s="15" t="str">
         <f t="shared" ref="A2:A23" si="0">CONCATENATE(C2,"/",B2)</f>
         <v>CodeSystem/urn:ietf:bcp:47</v>
@@ -27695,7 +27684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" s="3" customFormat="1">
       <c r="A3" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/CommonLanguages</v>
@@ -27719,7 +27708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" s="2" customFormat="1">
       <c r="A4" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/CompositionStatus</v>
@@ -27742,7 +27731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" s="3" customFormat="1">
       <c r="A5" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/ CompositionStatus</v>
@@ -27766,7 +27755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" s="2" customFormat="1">
       <c r="A6" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/http://loinc.org</v>
@@ -27788,7 +27777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" s="3" customFormat="1">
       <c r="A7" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/DocumentClassValueSet</v>
@@ -27811,7 +27800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" s="2" customFormat="1">
       <c r="A8" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/ResourceType</v>
@@ -27833,7 +27822,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" s="3" customFormat="1">
       <c r="A9" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/ResourceType</v>
@@ -27856,7 +27845,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" s="2" customFormat="1">
       <c r="A10" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/ v3.Confidentiality</v>
@@ -27878,7 +27867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" s="3" customFormat="1">
       <c r="A11" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/v3.ConfidentialityClassification</v>
@@ -27901,7 +27890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" s="2" customFormat="1">
       <c r="A12" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/CompositionAttestationMode</v>
@@ -27923,7 +27912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" s="3" customFormat="1">
       <c r="A13" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/CompositionAttestationMode</v>
@@ -27946,7 +27935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" s="2" customFormat="1">
       <c r="A14" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/DocumentRelationshipType</v>
@@ -27968,7 +27957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" s="3" customFormat="1">
       <c r="A15" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/DocumentRelationshipType</v>
@@ -27991,7 +27980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" s="2" customFormat="1">
       <c r="A16" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/v3-ActCode</v>
@@ -28013,7 +28002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" s="3" customFormat="1">
       <c r="A17" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/v3-ActCode</v>
@@ -28036,7 +28025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" s="2" customFormat="1">
       <c r="A18" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/v3-ActClass</v>
@@ -28058,7 +28047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" s="3" customFormat="1">
       <c r="A19" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/ 112 ValueSet</v>
@@ -28081,7 +28070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" s="2" customFormat="1">
       <c r="A20" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/http://loinc.org</v>
@@ -28103,7 +28092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" s="3" customFormat="1">
       <c r="A21" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/DocumentSectionCodes</v>
@@ -28126,7 +28115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" s="2" customFormat="1">
       <c r="A22" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/ListMode</v>
@@ -28149,7 +28138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" s="3" customFormat="1">
       <c r="A23" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/ListMode</v>
@@ -28173,7 +28162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" s="2" customFormat="1">
       <c r="A24" s="15" t="str">
         <f t="shared" ref="A24:A39" si="2">CONCATENATE(C24,"/",B24)</f>
         <v>CodeSystem/ListOrderCodes</v>
@@ -28196,7 +28185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" s="3" customFormat="1">
       <c r="A25" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/ListOrderCodes</v>
@@ -28220,7 +28209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" s="2" customFormat="1">
       <c r="A26" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/ListMode</v>
@@ -28243,7 +28232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" s="3" customFormat="1">
       <c r="A27" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/ListMode</v>
@@ -28267,7 +28256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" s="2" customFormat="1">
       <c r="A28" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/ListOrderCodes</v>
@@ -28289,7 +28278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" s="3" customFormat="1">
       <c r="A29" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/ListOrderCodes</v>
@@ -28312,7 +28301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" s="2" customFormat="1">
       <c r="A30" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/ListEmptyReasons</v>
@@ -28334,7 +28323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" s="3" customFormat="1">
       <c r="A31" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/ListEmptyReasons</v>
@@ -28357,7 +28346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" s="2" customFormat="1">
       <c r="A32" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/ListMode</v>
@@ -28379,7 +28368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" s="3" customFormat="1">
       <c r="A33" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/ListMode</v>
@@ -28402,7 +28391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" s="2" customFormat="1">
       <c r="A34" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/ListOrderCodes</v>
@@ -28424,7 +28413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" s="3" customFormat="1">
       <c r="A35" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/ListOrderCodes</v>
@@ -28447,7 +28436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" s="2" customFormat="1">
       <c r="A36" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/ListEmptyReasons</v>
@@ -28469,7 +28458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" s="3" customFormat="1">
       <c r="A37" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/ListEmptyReasons</v>
@@ -28492,7 +28481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" s="2" customFormat="1">
       <c r="A38" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/ListMode</v>
@@ -28514,7 +28503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" s="3" customFormat="1">
       <c r="A39" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/ListMode</v>
@@ -28537,7 +28526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" s="2" customFormat="1">
       <c r="A40" s="15" t="str">
         <f t="shared" ref="A40:A59" si="4">CONCATENATE(C40,"/",B40)</f>
         <v>CodeSystem/ListOrderCodes</v>
@@ -28559,7 +28548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" s="3" customFormat="1">
       <c r="A41" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/ListOrderCodes</v>
@@ -28582,7 +28571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" s="2" customFormat="1">
       <c r="A42" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/ListEmptyReasons</v>
@@ -28604,7 +28593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" s="3" customFormat="1">
       <c r="A43" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/ListEmptyReasons</v>
@@ -28627,7 +28616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" s="2" customFormat="1">
       <c r="A44" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/ListMode</v>
@@ -28649,7 +28638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" s="3" customFormat="1">
       <c r="A45" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/ListMode</v>
@@ -28672,7 +28661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" s="2" customFormat="1">
       <c r="A46" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/ListOrderCodes</v>
@@ -28694,7 +28683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" s="3" customFormat="1">
       <c r="A47" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/ListOrderCodes</v>
@@ -28717,7 +28706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" s="2" customFormat="1">
       <c r="A48" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/ListEmptyReasons</v>
@@ -28739,7 +28728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" s="3" customFormat="1">
       <c r="A49" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/ListEmptyReasons</v>
@@ -28762,7 +28751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" s="2" customFormat="1">
       <c r="A50" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/ListMode</v>
@@ -28784,7 +28773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" s="3" customFormat="1">
       <c r="A51" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/ListMode</v>
@@ -28807,7 +28796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" s="2" customFormat="1">
       <c r="A52" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/ListOrderCodes</v>
@@ -28829,7 +28818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" s="3" customFormat="1">
       <c r="A53" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/ListOrderCodes</v>
@@ -28852,7 +28841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" s="2" customFormat="1">
       <c r="A54" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/ListEmptyReasons</v>
@@ -28874,7 +28863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" s="3" customFormat="1">
       <c r="A55" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/ListEmptyReasons</v>
@@ -28897,7 +28886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" s="2" customFormat="1">
       <c r="A56" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/ListMode</v>
@@ -28919,7 +28908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" s="3" customFormat="1">
       <c r="A57" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/ListMode</v>
@@ -28942,7 +28931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" s="2" customFormat="1">
       <c r="A58" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/ListOrderCodes</v>
@@ -28964,7 +28953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" s="3" customFormat="1">
       <c r="A59" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/ListOrderCodes</v>
@@ -28987,7 +28976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" s="2" customFormat="1">
       <c r="A60" s="15" t="str">
         <f t="shared" ref="A60:A65" si="6">CONCATENATE(C60,"/",B60)</f>
         <v>CodeSystem/ListEmptyReasons</v>
@@ -29009,7 +28998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" s="3" customFormat="1">
       <c r="A61" s="14" t="str">
         <f t="shared" si="6"/>
         <v>ValueSet/ListEmptyReasons</v>
@@ -29032,7 +29021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" s="2" customFormat="1">
       <c r="A62" s="15" t="str">
         <f t="shared" si="6"/>
         <v>CodeSystem/ListMode</v>
@@ -29054,7 +29043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" s="3" customFormat="1">
       <c r="A63" s="14" t="str">
         <f t="shared" si="6"/>
         <v>ValueSet/ListMode</v>
@@ -29077,7 +29066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" s="2" customFormat="1">
       <c r="A64" s="15" t="str">
         <f t="shared" si="6"/>
         <v>CodeSystem/ListOrderCodes</v>
@@ -29099,7 +29088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" s="3" customFormat="1">
       <c r="A65" s="14" t="str">
         <f t="shared" si="6"/>
         <v>ValueSet/ListOrderCodes</v>
@@ -29122,7 +29111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" s="2" customFormat="1">
       <c r="A66" s="15" t="str">
         <f t="shared" ref="A66:A97" si="8">CONCATENATE(C66,"/",B66)</f>
         <v>CodeSystem/ListEmptyReasons</v>
@@ -29144,7 +29133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" s="3" customFormat="1">
       <c r="A67" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/ListEmptyReasons</v>
@@ -29167,7 +29156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" s="2" customFormat="1">
       <c r="A68" s="15" t="str">
         <f t="shared" si="8"/>
         <v>CodeSystem/ListMode</v>
@@ -29189,7 +29178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" s="3" customFormat="1">
       <c r="A69" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/ListMode</v>
@@ -29212,7 +29201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" s="2" customFormat="1">
       <c r="A70" s="15" t="str">
         <f t="shared" si="8"/>
         <v>CodeSystem/ListOrderCodes</v>
@@ -29234,7 +29223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" s="3" customFormat="1">
       <c r="A71" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/ListOrderCodes</v>
@@ -29257,7 +29246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" s="2" customFormat="1">
       <c r="A72" s="15" t="str">
         <f t="shared" si="8"/>
         <v>CodeSystem/ListEmptyReasons</v>
@@ -29279,7 +29268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" s="3" customFormat="1">
       <c r="A73" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/ListEmptyReasons</v>
@@ -29302,7 +29291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" s="2" customFormat="1">
       <c r="A74" s="15" t="str">
         <f t="shared" si="8"/>
         <v>CodeSystem/ListMode</v>
@@ -29324,7 +29313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" s="3" customFormat="1">
       <c r="A75" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/ListMode</v>
@@ -29347,7 +29336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" s="2" customFormat="1">
       <c r="A76" s="15" t="str">
         <f t="shared" si="8"/>
         <v>CodeSystem/ListOrderCodes</v>
@@ -29369,7 +29358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" s="3" customFormat="1">
       <c r="A77" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/ListOrderCodes</v>
@@ -29392,7 +29381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" s="2" customFormat="1">
       <c r="A78" s="15" t="str">
         <f t="shared" si="8"/>
         <v>CodeSystem/ListEmptyReasons</v>
@@ -29414,7 +29403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" s="3" customFormat="1">
       <c r="A79" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/ListEmptyReasons</v>
@@ -29437,7 +29426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" s="2" customFormat="1">
       <c r="A80" s="15" t="str">
         <f t="shared" si="8"/>
         <v>CodeSystem/ListMode</v>
@@ -29459,7 +29448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" s="3" customFormat="1">
       <c r="A81" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/ListMode</v>
@@ -29482,7 +29471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" s="2" customFormat="1">
       <c r="A82" s="15" t="str">
         <f t="shared" si="8"/>
         <v>CodeSystem/ListOrderCodes</v>
@@ -29504,7 +29493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" s="3" customFormat="1">
       <c r="A83" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/ListOrderCodes</v>
@@ -29527,7 +29516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" s="2" customFormat="1">
       <c r="A84" s="15" t="str">
         <f t="shared" si="8"/>
         <v>CodeSystem/ListEmptyReasons</v>
@@ -29549,7 +29538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" s="3" customFormat="1">
       <c r="A85" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/ListEmptyReasons</v>
@@ -29572,7 +29561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" s="2" customFormat="1">
       <c r="A86" s="15" t="str">
         <f t="shared" si="8"/>
         <v>CodeSystem/ListMode</v>
@@ -29594,7 +29583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" s="3" customFormat="1">
       <c r="A87" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/ListMode</v>
@@ -29617,7 +29606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" s="2" customFormat="1">
       <c r="A88" s="15" t="str">
         <f t="shared" si="8"/>
         <v>CodeSystem/ListOrderCodes</v>
@@ -29639,7 +29628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" s="3" customFormat="1">
       <c r="A89" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/ListOrderCodes</v>
@@ -29662,7 +29651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" s="2" customFormat="1">
       <c r="A90" s="15" t="str">
         <f t="shared" si="8"/>
         <v>CodeSystem/ListEmptyReasons</v>
@@ -29684,7 +29673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" s="3" customFormat="1">
       <c r="A91" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/ListEmptyReasons</v>
@@ -29707,7 +29696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" s="2" customFormat="1">
       <c r="A92" s="15" t="str">
         <f t="shared" si="8"/>
         <v>CodeSystem/ListMode</v>
@@ -29729,7 +29718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" s="3" customFormat="1">
       <c r="A93" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/ListMode</v>
@@ -29752,7 +29741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" s="2" customFormat="1">
       <c r="A94" s="15" t="str">
         <f t="shared" si="8"/>
         <v>CodeSystem/ListOrderCodes</v>
@@ -29774,7 +29763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" s="3" customFormat="1">
       <c r="A95" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/ListOrderCodes</v>
@@ -29797,7 +29786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" s="2" customFormat="1">
       <c r="A96" s="15" t="str">
         <f t="shared" si="8"/>
         <v>CodeSystem/ListEmptyReasons</v>
@@ -29819,7 +29808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" s="3" customFormat="1">
       <c r="A97" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/ListEmptyReasons</v>
@@ -29842,7 +29831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" s="2" customFormat="1">
       <c r="A98" s="15" t="str">
         <f t="shared" ref="A98:A103" si="10">CONCATENATE(C98,"/",B98)</f>
         <v>CodeSystem/ListMode</v>
@@ -29864,7 +29853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" s="3" customFormat="1">
       <c r="A99" s="14" t="str">
         <f t="shared" si="10"/>
         <v>ValueSet/ListMode</v>
@@ -29887,7 +29876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" s="2" customFormat="1">
       <c r="A100" s="15" t="str">
         <f t="shared" si="10"/>
         <v>CodeSystem/ListOrderCodes</v>
@@ -29909,7 +29898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" s="3" customFormat="1">
       <c r="A101" s="14" t="str">
         <f t="shared" si="10"/>
         <v>ValueSet/ListOrderCodes</v>
@@ -29932,7 +29921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" s="2" customFormat="1">
       <c r="A102" s="15" t="str">
         <f t="shared" si="10"/>
         <v>CodeSystem/ListEmptyReasons</v>
@@ -29954,7 +29943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" s="3" customFormat="1">
       <c r="A103" s="14" t="str">
         <f t="shared" si="10"/>
         <v>ValueSet/ListEmptyReasons</v>
@@ -29996,15 +29985,15 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="44.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -30030,7 +30019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="2" customFormat="1">
       <c r="A2" s="15" t="str">
         <f t="shared" ref="A2:A23" si="0">CONCATENATE(C2,"/",B2)</f>
         <v>CodeSystem/SearchEntryMode</v>
@@ -30053,7 +30042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" s="3" customFormat="1">
       <c r="A3" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -30077,7 +30066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" s="2" customFormat="1">
       <c r="A4" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -30100,7 +30089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" s="3" customFormat="1">
       <c r="A5" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/HTTPVerb</v>
@@ -30124,7 +30113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" s="2" customFormat="1">
       <c r="A6" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -30146,7 +30135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" s="3" customFormat="1">
       <c r="A7" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -30169,7 +30158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" s="2" customFormat="1">
       <c r="A8" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -30191,7 +30180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" s="3" customFormat="1">
       <c r="A9" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/HTTPVerb</v>
@@ -30214,7 +30203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" s="2" customFormat="1">
       <c r="A10" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -30236,7 +30225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" s="3" customFormat="1">
       <c r="A11" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -30259,7 +30248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" s="2" customFormat="1">
       <c r="A12" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -30281,7 +30270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" s="3" customFormat="1">
       <c r="A13" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/HTTPVerb</v>
@@ -30304,7 +30293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" s="2" customFormat="1">
       <c r="A14" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -30326,7 +30315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" s="3" customFormat="1">
       <c r="A15" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -30349,7 +30338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" s="2" customFormat="1">
       <c r="A16" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -30371,7 +30360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" s="3" customFormat="1">
       <c r="A17" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/HTTPVerb</v>
@@ -30394,7 +30383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" s="2" customFormat="1">
       <c r="A18" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -30416,7 +30405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" s="3" customFormat="1">
       <c r="A19" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -30439,7 +30428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" s="2" customFormat="1">
       <c r="A20" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -30461,7 +30450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" s="3" customFormat="1">
       <c r="A21" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/HTTPVerb</v>
@@ -30484,7 +30473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" s="2" customFormat="1">
       <c r="A22" s="15" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -30506,7 +30495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" s="3" customFormat="1">
       <c r="A23" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -30529,7 +30518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" s="2" customFormat="1">
       <c r="A24" s="15" t="str">
         <f t="shared" ref="A24:A51" si="2">CONCATENATE(C24,"/",B24)</f>
         <v>CodeSystem/HTTPVerb</v>
@@ -30552,7 +30541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" s="3" customFormat="1">
       <c r="A25" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/HTTPVerb</v>
@@ -30576,7 +30565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" s="2" customFormat="1">
       <c r="A26" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -30599,7 +30588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" s="3" customFormat="1">
       <c r="A27" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -30623,7 +30612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" s="2" customFormat="1">
       <c r="A28" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -30645,7 +30634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" s="3" customFormat="1">
       <c r="A29" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/HTTPVerb</v>
@@ -30668,7 +30657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" s="2" customFormat="1">
       <c r="A30" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -30690,7 +30679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" s="3" customFormat="1">
       <c r="A31" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -30713,7 +30702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" s="2" customFormat="1">
       <c r="A32" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -30735,7 +30724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" s="3" customFormat="1">
       <c r="A33" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/HTTPVerb</v>
@@ -30758,7 +30747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" s="2" customFormat="1">
       <c r="A34" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -30780,7 +30769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" s="3" customFormat="1">
       <c r="A35" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -30803,7 +30792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" s="2" customFormat="1">
       <c r="A36" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -30825,7 +30814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" s="3" customFormat="1">
       <c r="A37" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/HTTPVerb</v>
@@ -30848,7 +30837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" s="2" customFormat="1">
       <c r="A38" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -30870,7 +30859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" s="3" customFormat="1">
       <c r="A39" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -30893,7 +30882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" s="2" customFormat="1">
       <c r="A40" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -30915,7 +30904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" s="3" customFormat="1">
       <c r="A41" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/HTTPVerb</v>
@@ -30938,7 +30927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" s="2" customFormat="1">
       <c r="A42" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -30960,7 +30949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" s="3" customFormat="1">
       <c r="A43" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -30983,7 +30972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" s="2" customFormat="1">
       <c r="A44" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -31005,7 +30994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" s="3" customFormat="1">
       <c r="A45" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/HTTPVerb</v>
@@ -31028,7 +31017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" s="2" customFormat="1">
       <c r="A46" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -31050,7 +31039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" s="3" customFormat="1">
       <c r="A47" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -31073,7 +31062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" s="2" customFormat="1">
       <c r="A48" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -31095,7 +31084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" s="3" customFormat="1">
       <c r="A49" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/HTTPVerb</v>
@@ -31118,7 +31107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" s="2" customFormat="1">
       <c r="A50" s="15" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -31140,7 +31129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" s="3" customFormat="1">
       <c r="A51" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -31163,7 +31152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" s="2" customFormat="1">
       <c r="A52" s="15" t="str">
         <f t="shared" ref="A52:A75" si="4">CONCATENATE(C52,"/",B52)</f>
         <v>CodeSystem/HTTPVerb</v>
@@ -31186,7 +31175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" s="3" customFormat="1">
       <c r="A53" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/HTTPVerb</v>
@@ -31210,7 +31199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" s="2" customFormat="1">
       <c r="A54" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -31233,7 +31222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" s="3" customFormat="1">
       <c r="A55" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -31257,7 +31246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" s="2" customFormat="1">
       <c r="A56" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -31279,7 +31268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" s="3" customFormat="1">
       <c r="A57" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/HTTPVerb</v>
@@ -31302,7 +31291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" s="2" customFormat="1">
       <c r="A58" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -31324,7 +31313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" s="3" customFormat="1">
       <c r="A59" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -31347,7 +31336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" s="2" customFormat="1">
       <c r="A60" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -31369,7 +31358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" s="3" customFormat="1">
       <c r="A61" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/HTTPVerb</v>
@@ -31392,7 +31381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" s="2" customFormat="1">
       <c r="A62" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -31414,7 +31403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" s="3" customFormat="1">
       <c r="A63" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -31437,7 +31426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" s="2" customFormat="1">
       <c r="A64" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -31459,7 +31448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" s="3" customFormat="1">
       <c r="A65" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/HTTPVerb</v>
@@ -31482,7 +31471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" s="2" customFormat="1">
       <c r="A66" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -31504,7 +31493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" s="3" customFormat="1">
       <c r="A67" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -31527,7 +31516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" s="2" customFormat="1">
       <c r="A68" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -31549,7 +31538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" s="3" customFormat="1">
       <c r="A69" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/HTTPVerb</v>
@@ -31572,7 +31561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" s="2" customFormat="1">
       <c r="A70" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -31594,7 +31583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" s="3" customFormat="1">
       <c r="A71" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -31617,7 +31606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" s="2" customFormat="1">
       <c r="A72" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -31639,7 +31628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" s="3" customFormat="1">
       <c r="A73" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/HTTPVerb</v>
@@ -31662,7 +31651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" s="2" customFormat="1">
       <c r="A74" s="15" t="str">
         <f t="shared" si="4"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -31684,7 +31673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" s="3" customFormat="1">
       <c r="A75" s="14" t="str">
         <f t="shared" si="4"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -31707,7 +31696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" s="2" customFormat="1">
       <c r="A76" s="15" t="str">
         <f t="shared" ref="A76:A97" si="6">CONCATENATE(C76,"/",B76)</f>
         <v>CodeSystem/HTTPVerb</v>
@@ -31730,7 +31719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" s="3" customFormat="1">
       <c r="A77" s="14" t="str">
         <f t="shared" si="6"/>
         <v>ValueSet/HTTPVerb</v>
@@ -31754,7 +31743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" s="2" customFormat="1">
       <c r="A78" s="15" t="str">
         <f t="shared" si="6"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -31777,7 +31766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" s="3" customFormat="1">
       <c r="A79" s="14" t="str">
         <f t="shared" si="6"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -31801,7 +31790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" s="2" customFormat="1">
       <c r="A80" s="15" t="str">
         <f t="shared" si="6"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -31823,7 +31812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" s="3" customFormat="1">
       <c r="A81" s="14" t="str">
         <f t="shared" si="6"/>
         <v>ValueSet/HTTPVerb</v>
@@ -31846,7 +31835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" s="2" customFormat="1">
       <c r="A82" s="15" t="str">
         <f t="shared" si="6"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -31868,7 +31857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" s="3" customFormat="1">
       <c r="A83" s="14" t="str">
         <f t="shared" si="6"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -31891,7 +31880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" s="2" customFormat="1">
       <c r="A84" s="15" t="str">
         <f t="shared" si="6"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -31913,7 +31902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" s="3" customFormat="1">
       <c r="A85" s="14" t="str">
         <f t="shared" si="6"/>
         <v>ValueSet/HTTPVerb</v>
@@ -31936,7 +31925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" s="2" customFormat="1">
       <c r="A86" s="15" t="str">
         <f t="shared" si="6"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -31958,7 +31947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" s="3" customFormat="1">
       <c r="A87" s="14" t="str">
         <f t="shared" si="6"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -31981,7 +31970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" s="2" customFormat="1">
       <c r="A88" s="15" t="str">
         <f t="shared" si="6"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -32003,7 +31992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" s="3" customFormat="1">
       <c r="A89" s="14" t="str">
         <f t="shared" si="6"/>
         <v>ValueSet/HTTPVerb</v>
@@ -32026,7 +32015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" s="2" customFormat="1">
       <c r="A90" s="15" t="str">
         <f t="shared" si="6"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -32048,7 +32037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" s="3" customFormat="1">
       <c r="A91" s="14" t="str">
         <f t="shared" si="6"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -32071,7 +32060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" s="2" customFormat="1">
       <c r="A92" s="15" t="str">
         <f t="shared" si="6"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -32093,7 +32082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" s="3" customFormat="1">
       <c r="A93" s="14" t="str">
         <f t="shared" si="6"/>
         <v>ValueSet/HTTPVerb</v>
@@ -32116,7 +32105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" s="2" customFormat="1">
       <c r="A94" s="15" t="str">
         <f t="shared" si="6"/>
         <v>CodeSystem/SearchEntryMode</v>
@@ -32138,7 +32127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" s="3" customFormat="1">
       <c r="A95" s="14" t="str">
         <f t="shared" si="6"/>
         <v>ValueSet/SearchEntryMode</v>
@@ -32161,7 +32150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" s="2" customFormat="1">
       <c r="A96" s="15" t="str">
         <f t="shared" si="6"/>
         <v>CodeSystem/HTTPVerb</v>
@@ -32183,7 +32172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" s="3" customFormat="1">
       <c r="A97" s="14" t="str">
         <f t="shared" si="6"/>
         <v>ValueSet/HTTPVerb</v>
@@ -32206,7 +32195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" s="2" customFormat="1">
       <c r="A98" s="15" t="str">
         <f t="shared" ref="A98:A101" si="8">CONCATENATE(C98,"/",B98)</f>
         <v>CodeSystem/HTTPVerb</v>
@@ -32228,7 +32217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" s="3" customFormat="1">
       <c r="A99" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/HTTPVerb</v>
@@ -32251,7 +32240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" s="2" customFormat="1">
       <c r="A100" s="15" t="str">
         <f t="shared" si="8"/>
         <v>CodeSystem/</v>
@@ -32271,7 +32260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" s="3" customFormat="1">
       <c r="A101" s="14" t="str">
         <f t="shared" si="8"/>
         <v>ValueSet/</v>
@@ -32305,18 +32294,18 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="44.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -32348,7 +32337,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="2" customFormat="1">
       <c r="A2" s="2" t="str">
         <f>_xlfn.CONCAT(C2,"/",B2)</f>
         <v>CodeSystem/name-use</v>
@@ -32382,7 +32371,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="3" customFormat="1">
       <c r="A3" s="3" t="str">
         <f t="shared" ref="A3:A13" si="0">_xlfn.CONCAT(C3,"/",B3)</f>
         <v>ValueSet/name-use</v>
@@ -32416,7 +32405,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="2" customFormat="1">
       <c r="A4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/marital-status</v>
@@ -32450,7 +32439,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="3" customFormat="1">
       <c r="A5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/marital-status</v>
@@ -32484,7 +32473,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="2" customFormat="1">
       <c r="A6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/administrative-gender</v>
@@ -32518,7 +32507,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="3" customFormat="1">
       <c r="A7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/administrative-gender</v>
@@ -32552,7 +32541,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="3" customFormat="1">
       <c r="A8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/BRSexo-1.0</v>
@@ -32586,7 +32575,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="2" customFormat="1" ht="15.6">
       <c r="A9" s="2" t="s">
         <v>128</v>
       </c>
@@ -32619,7 +32608,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" s="3" customFormat="1">
       <c r="A10" s="3" t="str">
         <f>CONCATENATE(C10,"/",B10)</f>
         <v>ValueSet/patient-contactrelationship</v>
@@ -32653,7 +32642,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="2" customFormat="1">
       <c r="A11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/languages</v>
@@ -32687,7 +32676,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="3" customFormat="1">
       <c r="A12" s="3" t="str">
         <f>CONCATENATE(C12,"/",B12)</f>
         <v>CodeSystem/ietf-bcp-47</v>
@@ -32715,7 +32704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" s="2" customFormat="1">
       <c r="A13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/link-type</v>
@@ -32749,7 +32738,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" s="3" customFormat="1">
       <c r="A14" s="3" t="str">
         <f>CONCATENATE(C14,"/",B14)</f>
         <v>CodeSystem/link-type</v>
@@ -32783,7 +32772,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="2" customFormat="1" ht="15.6">
       <c r="A15" s="2" t="s">
         <v>124</v>
       </c>
@@ -32813,19 +32802,19 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" s="3" customFormat="1">
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="8:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="8:8" s="2" customFormat="1">
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="8:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="8:8" s="3" customFormat="1">
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="8:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="8:8" s="2" customFormat="1">
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="8:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="8:8" s="3" customFormat="1">
       <c r="H20" s="7"/>
     </row>
   </sheetData>
@@ -32841,17 +32830,17 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="44.6640625" customWidth="1"/>
-    <col min="5" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="5" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -32883,7 +32872,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="2" customFormat="1">
       <c r="A2" s="2" t="str">
         <f>_xlfn.CONCAT(C2,"/",B2)</f>
         <v>CodeSystem/organization-type</v>
@@ -32917,7 +32906,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="3" customFormat="1">
       <c r="A3" s="3" t="str">
         <f t="shared" ref="A3:A5" si="0">_xlfn.CONCAT(C3,"/",B3)</f>
         <v>ValueSet/organization-type</v>
@@ -32951,7 +32940,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="2" customFormat="1">
       <c r="A4" s="2" t="str">
         <f>_xlfn.CONCAT(C4,"/",B4)</f>
         <v>CodeSystem/BRTipoEstabelecimento</v>
@@ -32985,7 +32974,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="3" customFormat="1">
       <c r="A5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/BRTipoEstabelecimento</v>
@@ -33019,55 +33008,55 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="2" customFormat="1">
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="3" customFormat="1">
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="2" customFormat="1">
       <c r="A8" s="5" t="s">
         <v>83</v>
       </c>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="3" customFormat="1">
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" s="2" customFormat="1">
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="3" customFormat="1">
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="2" customFormat="1">
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" s="3" customFormat="1">
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" s="2" customFormat="1">
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="3" customFormat="1">
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" s="2" customFormat="1">
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="8:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="8:8" s="3" customFormat="1">
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="8:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="8:8" s="2" customFormat="1">
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="8:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="8:8" s="3" customFormat="1">
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="8:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="8:8" s="2" customFormat="1">
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="8:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="8:8" s="3" customFormat="1">
       <c r="H21" s="7"/>
     </row>
   </sheetData>
@@ -33083,18 +33072,18 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="44.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -33126,7 +33115,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="2" customFormat="1">
       <c r="A2" s="2" t="str">
         <f t="shared" ref="A2:A6" si="0">_xlfn.CONCAT(C2,"/",B2)</f>
         <v>CodeSystem/http://terminology.hl7.org/CodeSystem/v2-0360</v>
@@ -33157,7 +33146,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>138</v>
       </c>
@@ -33187,7 +33176,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="2" customFormat="1">
       <c r="A4" s="12" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/BRCBO</v>
@@ -33215,7 +33204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="3" customFormat="1">
       <c r="A5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/BRCBO-1.0</v>
@@ -33243,7 +33232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="2" customFormat="1">
       <c r="A6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ConceptMap/BRCBO</v>
@@ -33275,7 +33264,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="3" customFormat="1">
       <c r="H7" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -33303,17 +33292,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="44.6640625" customWidth="1"/>
-    <col min="5" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="5" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -33345,7 +33334,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="12" customFormat="1">
       <c r="A2" s="12" t="str">
         <f t="shared" ref="A2:A4" si="0">_xlfn.CONCAT(C2,"/",B2)</f>
         <v>ValueSet/https://build.fhir.org/ig/HL7/fhir-ips/ValueSet-healthcare-professional-roles-uv-ips.html</v>
@@ -33379,7 +33368,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="14" customFormat="1">
       <c r="A3" s="25" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/2.16.840.1.113883.2.9.6.2.7</v>
@@ -33413,7 +33402,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="12" customFormat="1">
       <c r="A4" s="12" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/http://hl7.org/fhir/ValueSet/c80-practice-codes</v>
@@ -33445,7 +33434,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="24" t="s">
         <v>83</v>
       </c>
@@ -33467,15 +33456,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="44.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -33498,7 +33487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -33509,7 +33498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>35</v>
       </c>
@@ -33520,7 +33509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="2" customFormat="1">
       <c r="A4" s="2" t="s">
         <v>34</v>
       </c>
@@ -33532,7 +33521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>35</v>
       </c>
@@ -33544,7 +33533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="2" customFormat="1">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -33553,7 +33542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="3" customFormat="1">
       <c r="A7" s="3" t="s">
         <v>35</v>
       </c>
@@ -33562,76 +33551,76 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="2" customFormat="1">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="3" customFormat="1">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="2" customFormat="1">
       <c r="A10" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" s="3" customFormat="1">
       <c r="A11" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="2" customFormat="1">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="3" customFormat="1">
       <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="2" customFormat="1">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="3" customFormat="1">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" s="2" customFormat="1">
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="7:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="7:7" s="3" customFormat="1">
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="7:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="7:7" s="2" customFormat="1">
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="7:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="7:7" s="3" customFormat="1">
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="7:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="7:7" s="2" customFormat="1">
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="7:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="7:7" s="3" customFormat="1">
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="7:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="7:7" s="2" customFormat="1">
       <c r="G22" s="6"/>
     </row>
-    <row r="23" spans="7:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="7:7" s="3" customFormat="1">
       <c r="G23" s="7"/>
     </row>
   </sheetData>
@@ -33643,20 +33632,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="44.6640625" customWidth="1"/>
-    <col min="5" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -33691,7 +33680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="2" customFormat="1">
       <c r="A2" s="2" t="str">
         <f t="shared" ref="A2:A14" si="0">CONCATENATE(C2,"/",B2)</f>
         <v>CodeSystem/AllergyIntoleranceClinicalStatusCodes</v>
@@ -33726,7 +33715,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="3" customFormat="1">
       <c r="A3" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/AllergyIntoleranceClinicalStatusCodes</v>
@@ -33761,7 +33750,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="2" customFormat="1">
       <c r="A4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/AllergyIntoleranceVerificationStatusCodes</v>
@@ -33795,7 +33784,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="3" customFormat="1">
       <c r="A5" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/AllergyIntoleranceVerificationStatusCodes</v>
@@ -33829,7 +33818,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="2" customFormat="1">
       <c r="A6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/AllergyIntoleranceType</v>
@@ -33863,7 +33852,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="3" customFormat="1">
       <c r="A7" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/AllergyIntoleranceType</v>
@@ -33897,7 +33886,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" s="2" customFormat="1">
       <c r="A8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/AllergyIntoleranceCategory</v>
@@ -33931,7 +33920,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" s="3" customFormat="1">
       <c r="A9" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/AllergyIntoleranceCategory</v>
@@ -33965,7 +33954,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" s="2" customFormat="1">
       <c r="A10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/AllergyIntoleranceCriticality</v>
@@ -33999,7 +33988,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" s="34" customFormat="1">
       <c r="A11" s="32" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/AllergyIntoleranceCriticality</v>
@@ -34033,7 +34022,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" s="3" customFormat="1">
       <c r="A12" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/Allergy Intolerance - SNOMED CT IPS Free Set</v>
@@ -34055,7 +34044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" s="2" customFormat="1">
       <c r="A13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>CodeSystem/Absent or Unknown Allergies - IPS</v>
@@ -34077,7 +34066,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" s="14" customFormat="1">
       <c r="A14" s="14" t="str">
         <f t="shared" si="0"/>
         <v>ValueSet/Absent or Unknown Allergies - IPS</v>
@@ -34101,7 +34090,7 @@
       </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" s="3" customFormat="1">
       <c r="A15" s="14" t="str">
         <f t="shared" ref="A15:A17" si="2">CONCATENATE(C15,"/",B15)</f>
         <v>ValueSet/AllergyReactionSnomedCtIpsFreeSet</v>
@@ -34123,7 +34112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" s="2" customFormat="1">
       <c r="A16" s="2" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/AllergyIntoleranceSeverity</v>
@@ -34145,7 +34134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="3" customFormat="1">
       <c r="A17" s="14" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/AllergyIntoleranceSeverity</v>
@@ -34174,24 +34163,23 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="53.33203125" customWidth="1"/>
-    <col min="2" max="2" width="37.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="28.1640625" customWidth="1"/>
-    <col min="5" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" style="40" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="37.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" style="40" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="43.2">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -34202,263 +34190,258 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>156</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="F1" s="37" t="s">
         <v>155</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="H1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="2" t="str">
         <f>CONCATENATE(C2,"/",B2)</f>
         <v>CodeSystem/HL7 event-status</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="20" t="s">
         <v>154</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="E2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="b">
+      <c r="F2" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="H2" s="6">
+        <f t="shared" ref="H2:H10" si="0">COUNTIF(D2:E2,TRUE)/COLUMNS(D2:E2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="18.600000000000001" customHeight="1">
+      <c r="A3" s="14" t="str">
+        <f t="shared" ref="A3:A10" si="1">CONCATENATE(C3,"/",B3)</f>
+        <v>ValueSet/HL7 ImmunizationStatusCodes</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>157</v>
-      </c>
-      <c r="H2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="6">
-        <f>COUNTIF(E2:F2,TRUE)/COLUMNS(E2:F2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="str">
-        <f t="shared" ref="A3:A10" si="0">CONCATENATE(C3,"/",B3)</f>
-        <v>ValueSet/HL7 ImmunizationStatusCodes</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>158</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="14" t="b">
+        <v>1</v>
+      </c>
       <c r="E3" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="14" t="b">
+      <c r="F3" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="7">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G3" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="7">
-        <f>COUNTIF(E3:F3,TRUE)/COLUMNS(E3:F3)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1">
       <c r="A4" s="2" t="str">
         <f>CONCATENATE(C4,"/",B4)</f>
         <v>ValueSet/HL7 Vaccines - SNOMED CT IPS Free Set</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>159</v>
+      <c r="B4" s="20" t="s">
+        <v>158</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="D4" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="E4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="38"/>
-      <c r="I4" s="6">
-        <f>COUNTIF(E4:F4,TRUE)/COLUMNS(E4:F4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="str">
+      <c r="F4" s="38"/>
+      <c r="H4" s="6">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="14" customFormat="1">
+      <c r="A5" s="14" t="str">
+        <f t="shared" si="1"/>
         <v>CodeSystem/ATC Vaccines WHO ATC - IPS</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="39"/>
+      <c r="H5" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="12" customFormat="1">
+      <c r="A6" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v>ValueSet/Vaccines WHO ATC - IPS</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="41"/>
+      <c r="G6" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="14" customFormat="1">
+      <c r="A7" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CodeSystem/Absent or Unknown Immunization - IPS</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="G7" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="12" customFormat="1">
+      <c r="A8" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v>ValueSet/HL7 body_site</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="41"/>
+      <c r="G8" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="14" customFormat="1">
+      <c r="A9" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>CodeSystem/http://standardterms.edqm.eu</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="38"/>
-      <c r="I5" s="10">
-        <f>COUNTIF(E5:F5,TRUE)/COLUMNS(E5:F5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="str">
+      <c r="D9" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="39"/>
+      <c r="G9" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="11">
         <f t="shared" si="0"/>
-        <v>ValueSet/Vaccines WHO ATC - IPS</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="12" customFormat="1" ht="15.6" customHeight="1">
+      <c r="A10" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v>ValueSet/MedicineRouteOfAdministrationUvIps</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="7">
-        <f>COUNTIF(E6:F6,TRUE)/COLUMNS(E6:F6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="str">
+      <c r="D10" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="G10" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="10">
         <f t="shared" si="0"/>
-        <v>CodeSystem/Absent or Unknown Immunization - IPS</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F7" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="H7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="10">
-        <f>COUNTIF(E7:F7,TRUE)/COLUMNS(E7:F7)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>ValueSet/HL7 body_site</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" s="39"/>
-      <c r="H8" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" s="7">
-        <f>COUNTIF(E8:F8,TRUE)/COLUMNS(E8:F8)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>CodeSystem/http://standardterms.edqm.eu</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" s="38"/>
-      <c r="H9" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I9" s="10">
-        <f>COUNTIF(E9:F9,TRUE)/COLUMNS(E9:F9)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>ValueSet/MedicineRouteOfAdministrationUvIps</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="H10" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" s="7">
-        <f>COUNTIF(E10:F10,TRUE)/COLUMNS(E10:F10)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:8" s="3" customFormat="1">
       <c r="A11" s="14" t="str">
-        <f t="shared" ref="A11" si="1">CONCATENATE(C11,"/",B11)</f>
+        <f t="shared" ref="A11" si="2">CONCATENATE(C11,"/",B11)</f>
         <v>ValueSet/VaccineTargetDiseasesUvIps</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -34467,65 +34450,68 @@
       <c r="C11" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="D11" s="14" t="b">
+        <v>0</v>
+      </c>
       <c r="E11" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="F11" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>164</v>
-      </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="7">
-        <f t="shared" ref="I11" si="2">COUNTIF(E11:F11,TRUE)/COLUMNS(E11:F11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F11" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="7">
+        <f t="shared" ref="H11" si="3">COUNTIF(D11:E11,TRUE)/COLUMNS(D11:E11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1">
       <c r="A12" s="2" t="str">
-        <f t="shared" ref="A12:A13" si="3">CONCATENATE(C12,"/",B12)</f>
+        <f t="shared" ref="A12:A13" si="4">CONCATENATE(C12,"/",B12)</f>
         <v>CodeSystem/</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D12" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="E12" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F12" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" s="38"/>
-      <c r="I12" s="10">
-        <f t="shared" ref="I12:I13" si="4">COUNTIF(E12:F12,TRUE)/COLUMNS(E12:F12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F12" s="38"/>
+      <c r="H12" s="10">
+        <f t="shared" ref="H12:H13" si="5">COUNTIF(D12:E12,TRUE)/COLUMNS(D12:E12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="3" customFormat="1">
       <c r="A13" s="14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>ValueSet/</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D13" s="14" t="b">
+        <v>0</v>
+      </c>
       <c r="E13" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="F13" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" s="39"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="7">
-        <f t="shared" si="4"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="7">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{50A2A781-3BB7-4D7B-B947-0269D4B0383E}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{B4191F2F-0ECF-4D7D-9187-6B12CC5C7E14}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{99409455-4B33-46C6-AE70-67F864A93199}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -34533,23 +34519,23 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="44.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="44.6640625" customWidth="1"/>
-    <col min="5" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="5" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -34575,88 +34561,86 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="2" customFormat="1">
       <c r="A2" s="2" t="str">
-        <f t="shared" ref="A2:A23" si="0">CONCATENATE(C2,"/",B2)</f>
-        <v>CodeSystem/urn:ietf:bcp:47</v>
+        <f t="shared" ref="A2:A21" si="0">CONCATENATE(C2,"/",B2)</f>
+        <v>CodeSystem/ConditionClinicalStatusCodes</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" s="6">
-        <f>COUNTIF(E2:F2,TRUE)/COLUMNS(E2:F2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="10">
+        <f t="shared" ref="H2:H21" si="1">COUNTIF(E2:F2,TRUE)/COLUMNS(E2:F2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1">
       <c r="A3" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>ValueSet/CommonLanguages</v>
+        <v>ValueSet/ConditionClinicalStatusCodes</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="7">
-        <f t="shared" ref="H3:H23" si="1">COUNTIF(E3:F3,TRUE)/COLUMNS(E3:F3)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1">
       <c r="A4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>CodeSystem/ConditionClinicalStatusCodes</v>
+        <v>CodeSystem/ConditionVerificationStatus</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5"/>
       <c r="E4" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" s="3" customFormat="1">
       <c r="A5" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>ValueSet/ConditionClinicalStatusCodes</v>
+        <v>ValueSet/ConditionVerificationStatus</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
       <c r="E5" s="14" t="b">
         <v>0</v>
       </c>
@@ -34669,13 +34653,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" s="2" customFormat="1">
       <c r="A6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>CodeSystem/ConditionVerificationStatus</v>
+        <v>CodeSystem/ ProblemTypeUvIps</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
@@ -34686,20 +34670,20 @@
       <c r="F6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" s="3" customFormat="1">
       <c r="A7" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>ValueSet/ConditionVerificationStatus</v>
+        <v>ValueSet/ ProblemTypeUvIps</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="14" t="b">
@@ -34714,15 +34698,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" s="2" customFormat="1">
       <c r="A8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>CodeSystem/ ProblemTypeUvIps</v>
+        <v>CodeSystem/Problem Type (LOINC)</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="2" t="b">
@@ -34736,15 +34720,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" s="3" customFormat="1">
       <c r="A9" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>ValueSet/ ProblemTypeUvIps</v>
+        <v>ValueSet/Problem Type (LOINC)</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="14" t="b">
@@ -34759,13 +34743,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" s="2" customFormat="1">
       <c r="A10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>CodeSystem/Problem Type (LOINC)</v>
+        <v>CodeSystem/Condition/DiagnosisSeverity</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>3</v>
@@ -34781,15 +34765,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" s="3" customFormat="1">
       <c r="A11" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>ValueSet/Problem Type (LOINC)</v>
+        <v>ValueSet/Condition/DiagnosisSeverity</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="14" t="b">
@@ -34804,15 +34788,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" s="2" customFormat="1">
       <c r="A12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>CodeSystem/Condition/DiagnosisSeverity</v>
+        <v>CodeSystem/Problem Severity - IPS</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="2" t="b">
@@ -34826,15 +34810,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" s="3" customFormat="1">
       <c r="A13" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>ValueSet/Condition/DiagnosisSeverity</v>
+        <v>ValueSet/Problem Severity - IPS</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="14" t="b">
@@ -34849,13 +34833,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" s="2" customFormat="1">
       <c r="A14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>CodeSystem/Problem Severity - IPS</v>
+        <v>CodeSystem/ProblemsSnomedAbsentUnknownUvIps</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>3</v>
@@ -34871,13 +34855,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" s="3" customFormat="1">
       <c r="A15" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>ValueSet/Problem Severity - IPS</v>
+        <v>ValueSet/ProblemsSnomedAbsentUnknownUvIps</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>4</v>
@@ -34894,13 +34878,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" s="2" customFormat="1">
       <c r="A16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>CodeSystem/ProblemsSnomedAbsentUnknownUvIps</v>
+        <v>CodeSystem/Problems - SNOMED CT IPS Free Set</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>3</v>
@@ -34916,13 +34900,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" s="3" customFormat="1">
       <c r="A17" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>ValueSet/ProblemsSnomedAbsentUnknownUvIps</v>
+        <v>ValueSet/Problems - SNOMED CT IPS Free Set</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>4</v>
@@ -34939,13 +34923,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" s="2" customFormat="1">
       <c r="A18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>CodeSystem/Problems - SNOMED CT IPS Free Set</v>
+        <v>CodeSystem/Absent or Unknown Problems - IPS</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>3</v>
@@ -34961,15 +34945,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" s="3" customFormat="1">
       <c r="A19" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>ValueSet/Problems - SNOMED CT IPS Free Set</v>
+        <v>ValueSet/Absent or Unknown Problems - IPS</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E19" s="14" t="b">
@@ -34984,13 +34968,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" s="2" customFormat="1">
       <c r="A20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>CodeSystem/Absent or Unknown Problems - IPS</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>56</v>
+        <v>CodeSystem/http://snomed.info/sct</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>74</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>3</v>
@@ -35006,15 +34990,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" s="3" customFormat="1">
       <c r="A21" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>ValueSet/Absent or Unknown Problems - IPS</v>
+        <v>ValueSet/SNOMEDCTBodyStructures</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E21" s="14" t="b">
@@ -35029,86 +35013,86 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" s="2" customFormat="1">
       <c r="A22" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>CodeSystem/http://snomed.info/sct</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>74</v>
+        <f t="shared" ref="A22:A27" si="2">CONCATENATE(C22,"/",B22)</f>
+        <v>CodeSystem/ResourceType</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H22" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="H22:H27" si="3">COUNTIF(E22:F22,TRUE)/COLUMNS(E22:F22)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="3" customFormat="1">
       <c r="A23" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>ValueSet/SNOMEDCTBodyStructures</v>
+        <f t="shared" si="2"/>
+        <v>ValueSet/ResourceType</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E23" s="14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="14" t="b">
         <v>0</v>
       </c>
       <c r="G23" s="14"/>
       <c r="H23" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="2" customFormat="1">
       <c r="A24" s="2" t="str">
-        <f t="shared" ref="A24:A29" si="2">CONCATENATE(C24,"/",B24)</f>
-        <v>CodeSystem/ResourceType</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>44</v>
+        <f t="shared" si="2"/>
+        <v>CodeSystem/http://snomed.info/sct</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>74</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H24" s="10">
-        <f t="shared" ref="H24:H29" si="3">COUNTIF(E24:F24,TRUE)/COLUMNS(E24:F24)</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="3" customFormat="1">
       <c r="A25" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>ValueSet/ResourceType</v>
+        <v>ValueSet/ ConditionStage</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="14" t="b">
         <v>0</v>
@@ -35116,10 +35100,10 @@
       <c r="G25" s="14"/>
       <c r="H25" s="7">
         <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="2" customFormat="1">
       <c r="A26" s="2" t="str">
         <f t="shared" si="2"/>
         <v>CodeSystem/http://snomed.info/sct</v>
@@ -35141,13 +35125,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" s="3" customFormat="1">
       <c r="A27" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>ValueSet/ ConditionStage</v>
+        <v>ValueSet/ConditionStageType</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>4</v>
@@ -35164,9 +35148,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" s="2" customFormat="1">
       <c r="A28" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A28:A31" si="4">CONCATENATE(C28,"/",B28)</f>
         <v>CodeSystem/http://snomed.info/sct</v>
       </c>
       <c r="B28" s="20" t="s">
@@ -35182,17 +35166,17 @@
         <v>0</v>
       </c>
       <c r="H28" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="H28:H31" si="5">COUNTIF(E28:F28,TRUE)/COLUMNS(E28:F28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="3" customFormat="1">
       <c r="A29" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>ValueSet/ConditionStageType</v>
+        <f t="shared" si="4"/>
+        <v>ValueSet/ManifestationAndSymptomCodes</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>4</v>
@@ -35205,17 +35189,14 @@
       </c>
       <c r="G29" s="14"/>
       <c r="H29" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="2" customFormat="1">
       <c r="A30" s="2" t="str">
-        <f t="shared" ref="A30:A33" si="4">CONCATENATE(C30,"/",B30)</f>
-        <v>CodeSystem/http://snomed.info/sct</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>74</v>
+        <f t="shared" si="4"/>
+        <v>CodeSystem/</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>3</v>
@@ -35227,17 +35208,14 @@
         <v>0</v>
       </c>
       <c r="H30" s="10">
-        <f t="shared" ref="H30:H33" si="5">COUNTIF(E30:F30,TRUE)/COLUMNS(E30:F30)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="3" customFormat="1">
       <c r="A31" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>ValueSet/ManifestationAndSymptomCodes</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>109</v>
+        <v>ValueSet/</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>4</v>
@@ -35254,51 +35232,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>CodeSystem/</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H32" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="14" t="str">
-        <f t="shared" si="4"/>
-        <v>ValueSet/</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F33" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="G33" s="14"/>
-      <c r="H33" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="B26" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-    <hyperlink ref="B28" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
-    <hyperlink ref="B30" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="B20" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="B24" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="B26" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="B28" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Planilhas de em CSV add
</commit_message>
<xml_diff>
--- a/Gestão do Projeto/Indicadores/SumarioIndicadores.xlsx
+++ b/Gestão do Projeto/Indicadores/SumarioIndicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syola\Documents\ips-brasil-documentos\Gestão do Projeto\Indicadores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D50AAE8-10EE-41BD-8FE9-A4FE280222A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A8A234-307C-4A0E-9D40-EBC1C2DA2EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sumario" sheetId="1" r:id="rId1"/>
@@ -25767,7 +25767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -29206,8 +29206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Ajuste no texto do sumário de indicadores
</commit_message>
<xml_diff>
--- a/Gestão do Projeto/Indicadores/SumarioIndicadores.xlsx
+++ b/Gestão do Projeto/Indicadores/SumarioIndicadores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GOInterop\git\ips-brasil-documentos\Gestão do Projeto\Indicadores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD314B2-299D-4402-87E2-554E3AF727D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562873C1-9555-4C86-9CF5-F432D5561D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sumario" sheetId="1" r:id="rId1"/>
@@ -868,8 +868,8 @@
   </si>
   <si>
     <t>TOTAL
-dos
-Modelos
+do
+Modelo
 Computacional</t>
   </si>
 </sst>
@@ -37174,8 +37174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37504,6 +37504,15 @@
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
+      <c r="G8" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="55" t="b">
+        <v>1</v>
+      </c>
       <c r="J8" s="144"/>
       <c r="K8" s="52" t="s">
         <v>37</v>
@@ -37572,6 +37581,15 @@
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
+      <c r="G10" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="55" t="b">
+        <v>1</v>
+      </c>
       <c r="J10" s="144"/>
       <c r="K10" s="52" t="s">
         <v>38</v>
@@ -37606,6 +37624,15 @@
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
+      <c r="G11" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="55" t="b">
+        <v>1</v>
+      </c>
       <c r="J11" s="144"/>
       <c r="K11" s="52" t="s">
         <v>72</v>
@@ -37706,6 +37733,15 @@
       </c>
       <c r="F14" s="53">
         <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G14" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="55" t="b">
         <v>1</v>
       </c>
       <c r="J14" s="144"/>

</xml_diff>

<commit_message>
casos de uso connectahton
</commit_message>
<xml_diff>
--- a/Gestão do Projeto/Indicadores/SumarioIndicadores.xlsx
+++ b/Gestão do Projeto/Indicadores/SumarioIndicadores.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/Documents/GitHub/ips-brasil-documentos/Gestão do Projeto/Indicadores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE8CCE1-88E5-3543-A6E1-E5599060D11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A79160-DD4D-FA48-A1AB-995948889C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20480" yWindow="6900" windowWidth="20480" windowHeight="12800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sumario" sheetId="1" r:id="rId1"/>
@@ -1481,10 +1481,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="20% - Ênfase1" xfId="2" builtinId="30"/>
-    <cellStyle name="40% - Ênfase1" xfId="3" builtinId="31"/>
-    <cellStyle name="Ênfase1" xfId="1" builtinId="29"/>
-    <cellStyle name="Hiperlink" xfId="4" builtinId="8"/>
+    <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -36969,7 +36969,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -42041,8 +42041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Sumario de indicadores atualizado
</commit_message>
<xml_diff>
--- a/Gestão do Projeto/Indicadores/SumarioIndicadores.xlsx
+++ b/Gestão do Projeto/Indicadores/SumarioIndicadores.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJET IPS\ips-brasil-documentos1\Gestão do Projeto\Indicadores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GOInterop\git\ips-brasil-documentos\Gestão do Projeto\Indicadores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD2202D-7582-46A5-8329-5588F3DAC2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D7803C-CC19-4420-BCE3-EB411FFBCF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sumario" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <sheet name="Bundle" sheetId="12" r:id="rId14"/>
     <sheet name="Specimen" sheetId="19" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="293">
   <si>
     <t>Artefato</t>
   </si>
@@ -876,12 +876,6 @@
     <t>Device</t>
   </si>
   <si>
-    <t>DeviceStatementUvIPS</t>
-  </si>
-  <si>
-    <t>DiagnosticReportUv</t>
-  </si>
-  <si>
     <t>Elemento Narrativo</t>
   </si>
   <si>
@@ -935,6 +929,12 @@
   </si>
   <si>
     <t>está faltando um código billing adddress http://hl7.org/fhir/R4/valueset-address-use.html</t>
+  </si>
+  <si>
+    <t>DeviceUseStatement</t>
+  </si>
+  <si>
+    <t>ImagingStudy</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1121,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -1465,12 +1465,21 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="20% - Ênfase1" xfId="2" builtinId="30"/>
-    <cellStyle name="40% - Ênfase1" xfId="3" builtinId="31"/>
-    <cellStyle name="Ênfase1" xfId="1" builtinId="29"/>
-    <cellStyle name="Hiperlink" xfId="4" builtinId="8"/>
+    <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -29451,7 +29460,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="15240" cy="209550"/>
@@ -29507,7 +29516,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="209550"/>
@@ -29563,7 +29572,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="15240" cy="209550"/>
@@ -29619,7 +29628,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="209550"/>
@@ -31355,7 +31364,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9525" cy="209550"/>
@@ -31411,7 +31420,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="209550"/>
@@ -31467,7 +31476,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9525" cy="209550"/>
@@ -31523,7 +31532,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="209550"/>
@@ -31579,7 +31588,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9525" cy="209550"/>
@@ -31635,7 +31644,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="209550"/>
@@ -31691,7 +31700,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9525" cy="209550"/>
@@ -31747,7 +31756,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="209550"/>
@@ -32251,7 +32260,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9525" cy="209550"/>
@@ -36955,7 +36964,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -37251,28 +37260,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.44140625" customWidth="1"/>
-    <col min="11" max="11" width="20.44140625" style="99" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" style="99" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="43.2">
+    <row r="1" spans="1:18" s="55" customFormat="1" ht="45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -37310,11 +37320,15 @@
       <c r="M1" s="75" t="s">
         <v>271</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>278</v>
-      </c>
+      <c r="N1" s="142" t="s">
+        <v>276</v>
+      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:14" s="55" customFormat="1">
+    <row r="2" spans="1:18" s="55" customFormat="1">
       <c r="A2" s="52" t="s">
         <v>32</v>
       </c>
@@ -37350,14 +37364,17 @@
       <c r="K2" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="53">
-        <v>1</v>
-      </c>
-      <c r="M2" s="53">
-        <v>1</v>
+      <c r="L2" s="149">
+        <v>1</v>
+      </c>
+      <c r="M2" s="149">
+        <v>1</v>
+      </c>
+      <c r="N2" s="149">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="55" customFormat="1">
+    <row r="3" spans="1:18" s="55" customFormat="1">
       <c r="A3" s="52" t="s">
         <v>33</v>
       </c>
@@ -37393,14 +37410,17 @@
       <c r="K3" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="53">
-        <v>1</v>
-      </c>
-      <c r="M3" s="53">
-        <v>1</v>
+      <c r="L3" s="149">
+        <v>1</v>
+      </c>
+      <c r="M3" s="149">
+        <v>1</v>
+      </c>
+      <c r="N3" s="149">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="55" customFormat="1">
+    <row r="4" spans="1:18" s="55" customFormat="1">
       <c r="A4" s="52" t="s">
         <v>34</v>
       </c>
@@ -37436,17 +37456,17 @@
       <c r="K4" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="L4" s="53">
-        <v>1</v>
-      </c>
-      <c r="M4" s="53">
-        <v>1</v>
-      </c>
-      <c r="N4" s="53">
+      <c r="L4" s="149">
+        <v>1</v>
+      </c>
+      <c r="M4" s="149">
+        <v>1</v>
+      </c>
+      <c r="N4" s="149">
         <v>0.7</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="55" customFormat="1">
+    <row r="5" spans="1:18" s="55" customFormat="1">
       <c r="A5" s="52" t="s">
         <v>35</v>
       </c>
@@ -37482,17 +37502,17 @@
       <c r="K5" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="55" t="s">
+      <c r="L5" s="150" t="s">
         <v>180</v>
       </c>
-      <c r="M5" s="55" t="s">
+      <c r="M5" s="150" t="s">
         <v>180</v>
       </c>
-      <c r="N5" s="53">
-        <v>0.2</v>
+      <c r="N5" s="149">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="55" customFormat="1">
+    <row r="6" spans="1:18" s="55" customFormat="1">
       <c r="A6" s="52" t="s">
         <v>74</v>
       </c>
@@ -37528,14 +37548,17 @@
       <c r="K6" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="L6" s="53" t="s">
-        <v>180</v>
-      </c>
-      <c r="M6" s="53">
-        <v>1</v>
+      <c r="L6" s="149">
+        <v>1</v>
+      </c>
+      <c r="M6" s="149">
+        <v>1</v>
+      </c>
+      <c r="N6" s="149">
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="55" customFormat="1">
+    <row r="7" spans="1:18" s="55" customFormat="1">
       <c r="A7" s="52" t="s">
         <v>36</v>
       </c>
@@ -37562,17 +37585,17 @@
       <c r="K7" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="L7" s="53">
-        <v>1</v>
-      </c>
-      <c r="M7" s="53">
-        <v>1</v>
-      </c>
-      <c r="N7" s="53">
+      <c r="L7" s="149">
+        <v>1</v>
+      </c>
+      <c r="M7" s="149">
+        <v>1</v>
+      </c>
+      <c r="N7" s="149">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="55" customFormat="1">
+    <row r="8" spans="1:18" s="55" customFormat="1">
       <c r="A8" s="52" t="s">
         <v>37</v>
       </c>
@@ -37608,14 +37631,17 @@
       <c r="K8" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="L8" s="53">
-        <v>1</v>
-      </c>
-      <c r="M8" s="53">
-        <v>1</v>
+      <c r="L8" s="149">
+        <v>1</v>
+      </c>
+      <c r="M8" s="149">
+        <v>1</v>
+      </c>
+      <c r="N8" s="149">
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="55" customFormat="1">
+    <row r="9" spans="1:18" s="55" customFormat="1">
       <c r="A9" s="52" t="s">
         <v>71</v>
       </c>
@@ -37642,14 +37668,17 @@
       <c r="K9" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="L9" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="M9" s="53">
-        <v>1</v>
+      <c r="L9" s="149">
+        <v>1</v>
+      </c>
+      <c r="M9" s="149">
+        <v>1</v>
+      </c>
+      <c r="N9" s="149">
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="55" customFormat="1">
+    <row r="10" spans="1:18" s="55" customFormat="1">
       <c r="A10" s="52" t="s">
         <v>38</v>
       </c>
@@ -37685,14 +37714,17 @@
       <c r="K10" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="L10" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="M10" s="53">
-        <v>1</v>
+      <c r="L10" s="149">
+        <v>1</v>
+      </c>
+      <c r="M10" s="149">
+        <v>1</v>
+      </c>
+      <c r="N10" s="149">
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="55" customFormat="1">
+    <row r="11" spans="1:18" s="55" customFormat="1">
       <c r="A11" s="52" t="s">
         <v>72</v>
       </c>
@@ -37728,14 +37760,17 @@
       <c r="K11" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="L11" s="53">
-        <v>1</v>
-      </c>
-      <c r="M11" s="53">
-        <v>1</v>
+      <c r="L11" s="149">
+        <v>1</v>
+      </c>
+      <c r="M11" s="149">
+        <v>1</v>
+      </c>
+      <c r="N11" s="149">
+        <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="55" customFormat="1">
+    <row r="12" spans="1:18" s="55" customFormat="1">
       <c r="A12" s="52" t="s">
         <v>39</v>
       </c>
@@ -37762,14 +37797,17 @@
       <c r="K12" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="L12" s="53">
-        <v>1</v>
-      </c>
-      <c r="M12" s="53">
-        <v>1</v>
+      <c r="L12" s="149">
+        <v>1</v>
+      </c>
+      <c r="M12" s="149">
+        <v>1</v>
+      </c>
+      <c r="N12" s="149">
+        <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="55" customFormat="1">
+    <row r="13" spans="1:18" s="55" customFormat="1">
       <c r="A13" s="52" t="s">
         <v>109</v>
       </c>
@@ -37796,14 +37834,17 @@
       <c r="K13" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="L13" s="53">
+      <c r="L13" s="149" t="s">
+        <v>180</v>
+      </c>
+      <c r="M13" s="149" t="s">
+        <v>180</v>
+      </c>
+      <c r="N13" s="149">
         <v>0</v>
       </c>
-      <c r="M13" s="53">
-        <v>0</v>
-      </c>
     </row>
-    <row r="14" spans="1:14" s="55" customFormat="1">
+    <row r="14" spans="1:18" s="55" customFormat="1">
       <c r="A14" s="52" t="s">
         <v>73</v>
       </c>
@@ -37839,14 +37880,17 @@
       <c r="K14" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="L14" s="53">
-        <v>1</v>
-      </c>
-      <c r="M14" s="53">
-        <v>1</v>
+      <c r="L14" s="149">
+        <v>1</v>
+      </c>
+      <c r="M14" s="149">
+        <v>1</v>
+      </c>
+      <c r="N14" s="149">
+        <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="1" customFormat="1" ht="57.6">
+    <row r="15" spans="1:18" customFormat="1" ht="60">
       <c r="A15" s="140" t="s">
         <v>274</v>
       </c>
@@ -37862,37 +37906,79 @@
         <f ca="1">AVERAGE(D2:D14)</f>
         <v>0.95002465483234722</v>
       </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="17">
         <f ca="1">AVERAGE(F2:F14)</f>
         <v>0.96482303309226392</v>
       </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
       <c r="J15" s="144"/>
-      <c r="K15" s="141" t="s">
+      <c r="K15" s="52" t="s">
+        <v>291</v>
+      </c>
+      <c r="L15" s="151">
+        <v>1</v>
+      </c>
+      <c r="M15" s="151">
+        <v>1</v>
+      </c>
+      <c r="N15" s="80" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="K16" s="52" t="s">
+        <v>275</v>
+      </c>
+      <c r="L16" s="151">
+        <v>1</v>
+      </c>
+      <c r="M16" s="151">
+        <v>1</v>
+      </c>
+      <c r="N16" s="80" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="11:18">
+      <c r="K17" s="52" t="s">
+        <v>292</v>
+      </c>
+      <c r="L17" s="150" t="s">
+        <v>180</v>
+      </c>
+      <c r="M17" s="150" t="s">
+        <v>180</v>
+      </c>
+      <c r="N17" s="80" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="11:18" ht="60">
+      <c r="K18" s="141" t="s">
         <v>273</v>
       </c>
-      <c r="L15" s="17">
+      <c r="L18" s="17">
         <f>AVERAGE(L2:L14)</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="M15" s="17">
+        <v>1</v>
+      </c>
+      <c r="M18" s="17">
         <f>AVERAGE(M2:M14)</f>
-        <v>0.91666666666666663</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="N18" s="17">
+        <f>AVERAGE(N2:N14)</f>
+        <v>0.13076923076923078</v>
+      </c>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
     </row>
-    <row r="17" spans="11:11">
-      <c r="K17" s="99" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="18" spans="11:11">
-      <c r="K18" s="99" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="19" spans="11:11">
-      <c r="K19" s="99" t="s">
-        <v>277</v>
-      </c>
+    <row r="1048576" spans="14:14">
+      <c r="N1048576" s="53"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -37935,17 +38021,17 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="46.33203125" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="6" width="11.6640625" style="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="80" customWidth="1"/>
-    <col min="8" max="9" width="8.6640625" style="80"/>
-    <col min="11" max="11" width="11.44140625" style="80" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.28515625" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="6" width="11.7109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="80" customWidth="1"/>
+    <col min="8" max="9" width="8.7109375" style="80"/>
+    <col min="11" max="11" width="11.42578125" style="80" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -38503,18 +38589,18 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="46.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="80" customWidth="1"/>
-    <col min="8" max="10" width="8.6640625" style="80"/>
-    <col min="11" max="11" width="11.6640625" style="80" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="80" customWidth="1"/>
+    <col min="8" max="10" width="8.7109375" style="80"/>
+    <col min="11" max="11" width="11.7109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -39179,17 +39265,17 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" style="80" customWidth="1"/>
-    <col min="12" max="12" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="80" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -40577,16 +40663,16 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
-    <col min="5" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -41427,16 +41513,16 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" customWidth="1"/>
-    <col min="5" max="6" width="11.6640625" style="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.6640625" style="80"/>
-    <col min="9" max="9" width="11.44140625" style="80" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="6" width="11.7109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.7109375" style="80"/>
+    <col min="9" max="9" width="11.42578125" style="80" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1">
@@ -41735,21 +41821,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53A93C4-FC73-4C85-9953-0A3238211A32}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -42033,21 +42119,21 @@
       <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.109375" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" style="41" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" style="41" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" style="41" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="41" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="41" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="41"/>
-    <col min="9" max="9" width="20.33203125" style="41" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" style="99"/>
-    <col min="11" max="11" width="13.33203125" style="99" customWidth="1"/>
-    <col min="12" max="12" width="58.109375" style="41" customWidth="1"/>
-    <col min="13" max="16384" width="8.6640625" style="41"/>
+    <col min="1" max="1" width="38.140625" style="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" style="41" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="41" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" style="41" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="41" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="41" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="41" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="41"/>
+    <col min="9" max="9" width="20.28515625" style="41" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="99"/>
+    <col min="11" max="11" width="13.28515625" style="99" customWidth="1"/>
+    <col min="12" max="12" width="58.140625" style="41" customWidth="1"/>
+    <col min="13" max="16384" width="8.7109375" style="41"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="25" customFormat="1">
@@ -42129,7 +42215,7 @@
       </c>
       <c r="L2" s="34"/>
       <c r="M2" s="34" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="28" customFormat="1">
@@ -42170,7 +42256,7 @@
       </c>
       <c r="L3" s="29"/>
       <c r="M3" s="29" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="33" customFormat="1">
@@ -42211,7 +42297,7 @@
       </c>
       <c r="L4" s="34"/>
       <c r="M4" s="34" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="33" customFormat="1">
@@ -42252,7 +42338,7 @@
       </c>
       <c r="L5" s="34"/>
       <c r="M5" s="34" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="28" customFormat="1">
@@ -42293,7 +42379,7 @@
       </c>
       <c r="L6" s="29"/>
       <c r="M6" s="29" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="33" customFormat="1">
@@ -42334,10 +42420,10 @@
       </c>
       <c r="L7" s="34"/>
       <c r="M7" s="34" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="28" customFormat="1" ht="230.4">
+    <row r="8" spans="1:13" s="28" customFormat="1" ht="240">
       <c r="A8" s="29" t="str">
         <f>CONCATENATE(C8,"/",B8)</f>
         <v>ValueSet/administrative-gender</v>
@@ -42418,10 +42504,10 @@
       </c>
       <c r="L9" s="29"/>
       <c r="M9" s="29" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="42" customFormat="1" ht="43.2">
+    <row r="10" spans="1:13" s="42" customFormat="1" ht="45">
       <c r="A10" s="39" t="s">
         <v>265</v>
       </c>
@@ -42458,10 +42544,10 @@
       </c>
       <c r="L10" s="44"/>
       <c r="M10" s="44" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="28" customFormat="1" ht="28.8">
+    <row r="11" spans="1:13" s="28" customFormat="1" ht="30">
       <c r="A11" s="29" t="str">
         <f>CONCATENATE(C11,"/",B11)</f>
         <v>ValueSet/RacaCategoriaBRIPS</v>
@@ -42493,7 +42579,7 @@
       <c r="K11" s="89"/>
       <c r="L11" s="38"/>
       <c r="M11" s="38" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="33" customFormat="1">
@@ -42530,7 +42616,7 @@
       <c r="K12" s="95"/>
       <c r="L12" s="34"/>
       <c r="M12" s="34" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="28" customFormat="1">
@@ -42569,7 +42655,7 @@
       </c>
       <c r="L13" s="29"/>
       <c r="M13" s="29" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="48" customFormat="1">
@@ -42610,7 +42696,7 @@
       </c>
       <c r="L14" s="32"/>
       <c r="M14" s="32" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="42" customFormat="1">
@@ -42651,7 +42737,7 @@
       </c>
       <c r="L15" s="39"/>
       <c r="M15" s="39" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="48" customFormat="1">
@@ -42692,7 +42778,7 @@
       </c>
       <c r="L16" s="32"/>
       <c r="M16" s="32" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" spans="1:13" s="42" customFormat="1">
@@ -42733,7 +42819,7 @@
       </c>
       <c r="L17" s="39"/>
       <c r="M17" s="39" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="50" customFormat="1">
@@ -42855,7 +42941,7 @@
       </c>
       <c r="L20" s="32"/>
       <c r="M20" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -42895,7 +42981,7 @@
         <v>180</v>
       </c>
       <c r="M21" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -43055,7 +43141,7 @@
         <v>180</v>
       </c>
       <c r="M25" s="148" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -43095,7 +43181,7 @@
         <v>180</v>
       </c>
       <c r="M26" s="148" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -43151,17 +43237,17 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" customWidth="1"/>
-    <col min="5" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" style="80"/>
-    <col min="11" max="11" width="11.44140625" style="80" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" customWidth="1"/>
+    <col min="5" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="80"/>
+    <col min="11" max="11" width="11.42578125" style="80" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -43554,19 +43640,19 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="57.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="27.44140625" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="80" customWidth="1"/>
-    <col min="9" max="10" width="8.6640625" style="80"/>
-    <col min="11" max="11" width="11.6640625" style="80" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="80" customWidth="1"/>
+    <col min="9" max="10" width="8.7109375" style="80"/>
+    <col min="11" max="11" width="11.7109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -43870,7 +43956,7 @@
       <c r="L8" s="102"/>
       <c r="M8" s="102"/>
     </row>
-    <row r="9" spans="1:13" s="28" customFormat="1" ht="18.45" customHeight="1">
+    <row r="9" spans="1:13" s="28" customFormat="1" ht="18.399999999999999" customHeight="1">
       <c r="A9" s="106" t="str">
         <f>CONCATENATE(C9,"/",B9)</f>
         <v>ValueSet/administrative-gender</v>
@@ -44014,16 +44100,16 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="6" width="11.6640625" style="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="80" customWidth="1"/>
-    <col min="8" max="10" width="8.6640625" style="80"/>
-    <col min="11" max="11" width="11.44140625" style="80" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="6" width="11.7109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="80" customWidth="1"/>
+    <col min="8" max="10" width="8.7109375" style="80"/>
+    <col min="11" max="11" width="11.42578125" style="80" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -44428,12 +44514,12 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
@@ -44608,16 +44694,16 @@
       <selection activeCell="M1" sqref="M1:N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="49.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="7" width="11.6640625" style="80" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="8.6640625" style="80"/>
-    <col min="11" max="11" width="11.6640625" style="80" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="7" width="11.7109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="8.7109375" style="80"/>
+    <col min="11" max="11" width="11.7109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
@@ -44696,7 +44782,7 @@
         <v>180</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="18" customFormat="1">
@@ -45063,7 +45149,7 @@
         <v>180</v>
       </c>
       <c r="M12" s="23" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="N12" s="145"/>
     </row>
@@ -45101,7 +45187,7 @@
         <v>121</v>
       </c>
       <c r="N13" s="146" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="13" customFormat="1">
@@ -45404,7 +45490,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="18" customFormat="1" ht="13.95" customHeight="1">
+    <row r="22" spans="1:13" s="18" customFormat="1" ht="13.9" customHeight="1">
       <c r="A22" s="18" t="str">
         <f t="shared" ref="A22" si="9">CONCATENATE(C22,"/",B22)</f>
         <v>ValueSet/BRCriticidadeAlergiasReacoesAdversas-1.0</v>
@@ -45478,7 +45564,7 @@
         <v>240</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:13" s="2" customFormat="1">
@@ -45518,7 +45604,7 @@
         <v>241</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="2" customFormat="1">
@@ -45555,10 +45641,10 @@
         <v>0</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="18" customFormat="1" ht="13.95" customHeight="1">
+    <row r="26" spans="1:13" s="18" customFormat="1" ht="13.9" customHeight="1">
       <c r="A26" s="18" t="str">
         <f>CONCATENATE(C26,"/",B26)</f>
         <v>ValueSet/BRAlergenos-1.0</v>
@@ -45592,7 +45678,7 @@
         <v>180</v>
       </c>
       <c r="M26" s="18" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -45637,17 +45723,17 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="53.33203125" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" customWidth="1"/>
-    <col min="3" max="4" width="14.109375" customWidth="1"/>
-    <col min="5" max="6" width="11.6640625" style="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="80" customWidth="1"/>
-    <col min="8" max="10" width="8.6640625" style="80"/>
-    <col min="11" max="11" width="11.6640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="3" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="6" width="11.7109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="80" customWidth="1"/>
+    <col min="8" max="10" width="8.7109375" style="80"/>
+    <col min="11" max="11" width="11.7109375" style="80" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21" style="80" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
@@ -45800,7 +45886,7 @@
       </c>
       <c r="L4" s="132"/>
     </row>
-    <row r="5" spans="1:14" s="18" customFormat="1" ht="16.95" customHeight="1">
+    <row r="5" spans="1:14" s="18" customFormat="1" ht="16.899999999999999" customHeight="1">
       <c r="A5" s="12" t="str">
         <f t="shared" ref="A5:A25" si="2">CONCATENATE(C5,"/",B5)</f>
         <v>ValueSet/immunization-status</v>
@@ -45834,7 +45920,7 @@
       </c>
       <c r="L5" s="86"/>
     </row>
-    <row r="6" spans="1:14" s="18" customFormat="1" ht="16.95" customHeight="1">
+    <row r="6" spans="1:14" s="18" customFormat="1" ht="16.899999999999999" customHeight="1">
       <c r="A6" s="12" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/vaccines-uv-ips</v>
@@ -46087,7 +46173,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="18" customFormat="1" ht="15.45" customHeight="1">
+    <row r="13" spans="1:14" s="18" customFormat="1" ht="15.4" customHeight="1">
       <c r="A13" s="12" t="str">
         <f t="shared" si="2"/>
         <v>ValueSet/MedicineRouteOfAdministrationUvIps</v>
@@ -46599,17 +46685,17 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="80" customWidth="1"/>
-    <col min="8" max="10" width="8.6640625" style="80"/>
-    <col min="11" max="11" width="11.6640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="80" customWidth="1"/>
+    <col min="8" max="10" width="8.7109375" style="80"/>
+    <col min="11" max="11" width="11.7109375" style="80" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>